<commit_message>
new data time stamps
</commit_message>
<xml_diff>
--- a/data/lab_2_paperweights.xlsx
+++ b/data/lab_2_paperweights.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wlperry/Documents/r_projects/eco_201_labs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C08112-2203-7041-B09A-BE7ABEB4B9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD65FE8-1B0F-8343-8615-DD6E09D10DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="53740" yWindow="600" windowWidth="28100" windowHeight="17440" xr2:uid="{B84C37D2-62A9-7C42-AF78-A8F5ABF99D11}"/>
   </bookViews>
@@ -415,7 +415,7 @@
   <dimension ref="A1:B119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:B119"/>
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -430,178 +430,178 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>3.1899999999999998E-2</v>
+        <v>4.8999999999999998E-3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>3.0200000000000001E-2</v>
+        <v>5.1999999999999998E-3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>3.15E-2</v>
+        <v>5.7999999999999996E-3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>3.1899999999999998E-2</v>
+        <v>5.8999999999999999E-3</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>2.7799999999999998E-2</v>
+        <v>6.1000000000000004E-3</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>3.1899999999999998E-2</v>
+        <v>6.1999999999999998E-3</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B8">
-        <v>3.3000000000000002E-2</v>
+        <v>6.3E-3</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B9">
-        <v>3.0599999999999999E-2</v>
+        <v>6.4000000000000003E-3</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B10">
-        <v>0.124</v>
+        <v>6.4999999999999997E-3</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B11">
-        <v>0.1205</v>
+        <v>6.6E-3</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B12">
-        <v>0.1245</v>
+        <v>6.6E-3</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B13">
-        <v>0.124</v>
+        <v>6.7000000000000002E-3</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B14">
-        <v>0.1206</v>
+        <v>6.7000000000000002E-3</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="B15">
-        <v>0.27100000000000002</v>
+        <v>6.7000000000000002E-3</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="B16">
-        <v>0.27060000000000001</v>
+        <v>6.7000000000000002E-3</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="B17">
-        <v>0.26629999999999998</v>
+        <v>6.7999999999999996E-3</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="B18">
-        <v>0.75049999999999994</v>
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="B19">
-        <v>0.78010000000000002</v>
+        <v>7.3000000000000001E-3</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>225</v>
+        <v>1</v>
       </c>
       <c r="B20">
-        <v>1.7370000000000001</v>
+        <v>7.4999999999999997E-3</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>400</v>
+        <v>1</v>
       </c>
       <c r="B21">
-        <v>3.0950000000000002</v>
+        <v>7.6E-3</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>400</v>
+        <v>1</v>
       </c>
       <c r="B22">
-        <v>3.0615000000000001</v>
+        <v>7.6E-3</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>500</v>
+        <v>1</v>
       </c>
       <c r="B23">
-        <v>3.7719999999999998</v>
+        <v>7.6E-3</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -609,7 +609,7 @@
         <v>1</v>
       </c>
       <c r="B24">
-        <v>4.8999999999999998E-3</v>
+        <v>8.2000000000000007E-3</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -617,7 +617,7 @@
         <v>1</v>
       </c>
       <c r="B25">
-        <v>5.1999999999999998E-3</v>
+        <v>8.2000000000000007E-3</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -625,183 +625,183 @@
         <v>1</v>
       </c>
       <c r="B26">
-        <v>5.7999999999999996E-3</v>
+        <v>8.2000000000000007E-3</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B27">
-        <v>5.8999999999999999E-3</v>
+        <v>3.1899999999999998E-2</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B28">
-        <v>6.1000000000000004E-3</v>
+        <v>3.0200000000000001E-2</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B29">
-        <v>6.1999999999999998E-3</v>
+        <v>3.15E-2</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B30">
-        <v>6.3E-3</v>
+        <v>3.1899999999999998E-2</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B31">
-        <v>6.4000000000000003E-3</v>
+        <v>2.7799999999999998E-2</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B32">
-        <v>6.4999999999999997E-3</v>
+        <v>3.1899999999999998E-2</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B33">
-        <v>6.6E-3</v>
+        <v>3.3000000000000002E-2</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B34">
-        <v>6.6E-3</v>
+        <v>3.0599999999999999E-2</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B35">
-        <v>6.7000000000000002E-3</v>
+        <v>2.7799999999999998E-2</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B36">
-        <v>6.7000000000000002E-3</v>
+        <v>2.81E-2</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B37">
-        <v>6.7000000000000002E-3</v>
+        <v>2.81E-2</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B38">
-        <v>6.7000000000000002E-3</v>
+        <v>2.8500000000000001E-2</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B39">
-        <v>6.7999999999999996E-3</v>
+        <v>2.86E-2</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B40">
-        <v>7.0000000000000001E-3</v>
+        <v>2.86E-2</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B41">
-        <v>7.3000000000000001E-3</v>
+        <v>2.87E-2</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B42">
-        <v>7.4999999999999997E-3</v>
+        <v>2.8799999999999999E-2</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B43">
-        <v>7.6E-3</v>
+        <v>2.8899999999999999E-2</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B44">
-        <v>7.6E-3</v>
+        <v>2.92E-2</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B45">
-        <v>7.6E-3</v>
+        <v>2.93E-2</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B46">
-        <v>8.2000000000000007E-3</v>
+        <v>2.9399999999999999E-2</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B47">
-        <v>8.2000000000000007E-3</v>
+        <v>2.9499999999999998E-2</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B48">
-        <v>8.2000000000000007E-3</v>
+        <v>2.9600000000000001E-2</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -809,7 +809,7 @@
         <v>4</v>
       </c>
       <c r="B49">
-        <v>2.7799999999999998E-2</v>
+        <v>2.9600000000000001E-2</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -817,7 +817,7 @@
         <v>4</v>
       </c>
       <c r="B50">
-        <v>2.81E-2</v>
+        <v>2.9700000000000001E-2</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -825,7 +825,7 @@
         <v>4</v>
       </c>
       <c r="B51">
-        <v>2.81E-2</v>
+        <v>2.98E-2</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -833,7 +833,7 @@
         <v>4</v>
       </c>
       <c r="B52">
-        <v>2.8500000000000001E-2</v>
+        <v>2.9899999999999999E-2</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -841,7 +841,7 @@
         <v>4</v>
       </c>
       <c r="B53">
-        <v>2.86E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -849,7 +849,7 @@
         <v>4</v>
       </c>
       <c r="B54">
-        <v>2.86E-2</v>
+        <v>3.0300000000000001E-2</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -857,7 +857,7 @@
         <v>4</v>
       </c>
       <c r="B55">
-        <v>2.87E-2</v>
+        <v>3.0700000000000002E-2</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -865,7 +865,7 @@
         <v>4</v>
       </c>
       <c r="B56">
-        <v>2.8799999999999999E-2</v>
+        <v>3.09E-2</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -873,7 +873,7 @@
         <v>4</v>
       </c>
       <c r="B57">
-        <v>2.8899999999999999E-2</v>
+        <v>3.15E-2</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -881,119 +881,119 @@
         <v>4</v>
       </c>
       <c r="B58">
-        <v>2.92E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B59">
-        <v>2.93E-2</v>
+        <v>0.124</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B60">
-        <v>2.9399999999999999E-2</v>
+        <v>0.1205</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B61">
-        <v>2.9499999999999998E-2</v>
+        <v>0.1245</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B62">
-        <v>2.9600000000000001E-2</v>
+        <v>0.124</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B63">
-        <v>2.9600000000000001E-2</v>
+        <v>0.1206</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B64">
-        <v>2.9700000000000001E-2</v>
+        <v>0.1159</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B65">
-        <v>2.98E-2</v>
+        <v>0.11609999999999999</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B66">
-        <v>2.9899999999999999E-2</v>
+        <v>0.1166</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B67">
-        <v>0.03</v>
+        <v>0.1169</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B68">
-        <v>3.0300000000000001E-2</v>
+        <v>0.11749999999999999</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B69">
-        <v>3.0700000000000002E-2</v>
+        <v>0.1182</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B70">
-        <v>3.09E-2</v>
+        <v>0.11849999999999999</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B71">
-        <v>3.15E-2</v>
+        <v>0.11849999999999999</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B72">
-        <v>3.2000000000000001E-2</v>
+        <v>0.1201</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1001,7 +1001,7 @@
         <v>16</v>
       </c>
       <c r="B73">
-        <v>0.1159</v>
+        <v>0.12039999999999999</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1009,7 +1009,7 @@
         <v>16</v>
       </c>
       <c r="B74">
-        <v>0.11609999999999999</v>
+        <v>0.1212</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1017,7 +1017,7 @@
         <v>16</v>
       </c>
       <c r="B75">
-        <v>0.1166</v>
+        <v>0.1216</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1025,7 +1025,7 @@
         <v>16</v>
       </c>
       <c r="B76">
-        <v>0.1169</v>
+        <v>0.1217</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1033,7 +1033,7 @@
         <v>16</v>
       </c>
       <c r="B77">
-        <v>0.11749999999999999</v>
+        <v>0.12189999999999999</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1041,7 +1041,7 @@
         <v>16</v>
       </c>
       <c r="B78">
-        <v>0.1182</v>
+        <v>0.1226</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1049,7 +1049,7 @@
         <v>16</v>
       </c>
       <c r="B79">
-        <v>0.11849999999999999</v>
+        <v>0.1229</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1057,7 +1057,7 @@
         <v>16</v>
       </c>
       <c r="B80">
-        <v>0.11849999999999999</v>
+        <v>0.1235</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1065,7 +1065,7 @@
         <v>16</v>
       </c>
       <c r="B81">
-        <v>0.1201</v>
+        <v>0.1237</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1073,79 +1073,79 @@
         <v>16</v>
       </c>
       <c r="B82">
-        <v>0.12039999999999999</v>
+        <v>0.12540000000000001</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B83">
-        <v>0.1212</v>
+        <v>0.27100000000000002</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B84">
-        <v>0.1216</v>
+        <v>0.27060000000000001</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B85">
-        <v>0.1217</v>
+        <v>0.26629999999999998</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="B86">
-        <v>0.12189999999999999</v>
+        <v>0.47820000000000001</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="B87">
-        <v>0.1226</v>
+        <v>0.47839999999999999</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="B88">
-        <v>0.1229</v>
+        <v>0.47989999999999999</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="B89">
-        <v>0.1235</v>
+        <v>0.48020000000000002</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="B90">
-        <v>0.1237</v>
+        <v>0.48039999999999999</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="B91">
-        <v>0.12540000000000001</v>
+        <v>0.49340000000000001</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1153,55 +1153,55 @@
         <v>64</v>
       </c>
       <c r="B92">
-        <v>0.47820000000000001</v>
+        <v>0.49609999999999999</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="B93">
-        <v>0.47839999999999999</v>
+        <v>0.75049999999999994</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="B94">
-        <v>0.47989999999999999</v>
+        <v>0.78010000000000002</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="B95">
-        <v>0.48020000000000002</v>
+        <v>0.74029999999999996</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="B96">
-        <v>0.48039999999999999</v>
+        <v>0.74719999999999998</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="B97">
-        <v>0.49340000000000001</v>
+        <v>0.75080000000000002</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="B98">
-        <v>0.49609999999999999</v>
+        <v>0.75149999999999995</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1209,7 +1209,7 @@
         <v>100</v>
       </c>
       <c r="B99">
-        <v>0.74029999999999996</v>
+        <v>0.75249999999999995</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1217,7 +1217,7 @@
         <v>100</v>
       </c>
       <c r="B100">
-        <v>0.74719999999999998</v>
+        <v>0.75849999999999995</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1225,7 +1225,7 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>0.75080000000000002</v>
+        <v>0.76039999999999996</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1233,7 +1233,7 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>0.75149999999999995</v>
+        <v>0.76160000000000005</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1241,7 +1241,7 @@
         <v>100</v>
       </c>
       <c r="B103">
-        <v>0.75249999999999995</v>
+        <v>0.76290000000000002</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1249,7 +1249,7 @@
         <v>100</v>
       </c>
       <c r="B104">
-        <v>0.75849999999999995</v>
+        <v>0.77059999999999995</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1257,7 +1257,7 @@
         <v>100</v>
       </c>
       <c r="B105">
-        <v>0.76039999999999996</v>
+        <v>0.77170000000000005</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1265,39 +1265,39 @@
         <v>100</v>
       </c>
       <c r="B106">
-        <v>0.76160000000000005</v>
+        <v>0.77680000000000005</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107">
-        <v>100</v>
+        <v>225</v>
       </c>
       <c r="B107">
-        <v>0.76290000000000002</v>
+        <v>1.7370000000000001</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="B108">
-        <v>0.77059999999999995</v>
+        <v>3.0950000000000002</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="B109">
-        <v>0.77170000000000005</v>
+        <v>3.0615000000000001</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="B110">
-        <v>0.77680000000000005</v>
+        <v>3.0225</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1305,7 +1305,7 @@
         <v>400</v>
       </c>
       <c r="B111">
-        <v>3.0225</v>
+        <v>3.0516999999999999</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1313,7 +1313,7 @@
         <v>400</v>
       </c>
       <c r="B112">
-        <v>3.0516999999999999</v>
+        <v>3.0630000000000002</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1321,15 +1321,15 @@
         <v>400</v>
       </c>
       <c r="B113">
-        <v>3.0630000000000002</v>
+        <v>3.1181999999999999</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="B114">
-        <v>3.1181999999999999</v>
+        <v>3.7719999999999998</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1378,6 +1378,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B119">
+    <sortCondition ref="A2:A119"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>